<commit_message>
Start of day 3 part 2
</commit_message>
<xml_diff>
--- a/2017/day3_2.xlsx
+++ b/2017/day3_2.xlsx
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,127 +111,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B11:G16"/>
+  <dimension ref="L16:Q21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="0" t="n">
-        <f aca="false">G12+F12</f>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q16" s="0" t="n">
+        <f aca="false">Q17+P17</f>
         <v>2398</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L17" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="M17" s="0" t="n">
         <v>142</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="N17" s="0" t="n">
         <v>133</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="O17" s="0" t="n">
         <v>122</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="P17" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">G13+F13+F12</f>
+      <c r="Q17" s="0" t="n">
+        <f aca="false">Q18+P18+P17</f>
         <v>2339</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L18" s="0" t="n">
         <v>304</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="M18" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="N18" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="O18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="P18" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">G14+F14+F13+F12</f>
+      <c r="Q18" s="0" t="n">
+        <f aca="false">Q19+P19+P18+P17</f>
         <v>2223</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L19" s="0" t="n">
         <v>330</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="M19" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="N19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="O19" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="P19" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">G15+F15+F14+F13</f>
+      <c r="Q19" s="0" t="n">
+        <f aca="false">Q20+P20+P19+P18</f>
         <v>2053</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L20" s="0" t="n">
         <v>351</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="M20" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="N20" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="O20" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="P20" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">G16+F16+F15+F14</f>
+      <c r="Q20" s="0" t="n">
+        <f aca="false">Q21+P21+P20+P19</f>
         <v>1916</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L21" s="0" t="n">
         <v>362</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="M21" s="0" t="n">
         <v>747</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="N21" s="0" t="n">
         <v>806</v>
       </c>
-      <c r="E16" s="0" t="n">
-        <f aca="false">D16+D15+E15</f>
+      <c r="O21" s="0" t="n">
+        <f aca="false">N21+N20+O20</f>
         <v>854</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <f aca="false">E16+E15+F15</f>
+      <c r="P21" s="0" t="n">
+        <f aca="false">O21+O20+P20</f>
         <v>905</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <f aca="false">F16+F15</f>
+      <c r="Q21" s="0" t="n">
+        <f aca="false">P21+P20</f>
         <v>931</v>
       </c>
     </row>

</xml_diff>